<commit_message>
short water ecoinvent 14
</commit_message>
<xml_diff>
--- a/data/Water_database_38.xlsx
+++ b/data/Water_database_38.xlsx
@@ -527,7 +527,7 @@
   <dimension ref="A1:AC120"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="109" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -546,7 +546,7 @@
         <v>0</v>
       </c>
       <c r="B1">
-        <v>1</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.3">

</xml_diff>